<commit_message>
forgot to commit lol
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0f92f3d012b9fa0/Documents/Senior_Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC104888095C45085BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD51F0DD-EFD3-4892-87BB-0BC8E2728AFA}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="11_F25DC773A252ABDACC104888095C45085BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB79DEF6-327E-4903-B2A1-1F3AAF055016}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="12300" yWindow="1764" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="Wishlist1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Part</t>
   </si>
@@ -112,16 +124,81 @@
   </si>
   <si>
     <t>Assorted wires and hardware</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bumpers  #6835 &amp; Rear #6836 Bumpers Skid Plate with Mounts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sincecam 50KG Brushless Servo Motor 180° Steering Servo Magnetic Metal Gear 1/10 Waterproof </t>
+  </si>
+  <si>
+    <t>Sincecam 50kg 12.6V Brushless Servo 3S High Voltage Battery Power Adapter</t>
+  </si>
+  <si>
+    <t>Portable Charger 38800mAh,LCD Display Power Bank,4 USB Outputs Battery Pack Backup</t>
+  </si>
+  <si>
+    <t>Buying Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVIDIA Jetson Orin Nano Developer Kit </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Bumpers-Compatible-Traxxas-Platinum-Mounts/dp/B093D1GCLY/ref=sr_1_3?keywords=traxxas+slash+bumper&amp;qid=1695671541&amp;sr=8-3</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Sincecam-Brushless-Steering-Induction-Waterproof/dp/B0BMVKHZPJ?th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Sincecam-Brushless-Voltage-Suitable-SC1250MGX/dp/B0BMVW5DXJ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Portable-Charger-38800mAh-Charging-Compatible/dp/B09H4GLZXT/ref=sr_1_14?crid=2GYOFTLDQMXKP&amp;keywords=usb%2Bpower%2Bbank%2B3a%2Boutput&amp;qid=1695672928&amp;sprefix=usb%2Bpower%2Bbank%2B3a%2Boutput%2Caps%2C129&amp;sr=8-14&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0BZJTQ5YP?th=1</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,13 +221,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -164,6 +249,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,4 +689,113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDA9047-491B-480A-8180-AAE4D3FC6C29}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="85.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2">
+        <v>81.97</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8.99</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2">
+        <v>25.95</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2">
+        <v>499.99</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <f>SUM(B1:B6)</f>
+        <v>636.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{5AF121C0-563A-4D69-B9EF-117D69B41D88}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{66A011DD-D960-44D4-891B-5E1FD2FA97BB}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{B65FDA4E-F923-4EA6-9DC9-A8A6BC57C369}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{E26652DD-8F62-453A-8DF9-03244682A196}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{385A6503-C13C-4F34-8836-BB3EDD15AA1A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more POs and journals
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0f92f3d012b9fa0/Documents/Senior_Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="11_F25DC773A252ABDACC104888095C45085BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{324AB39D-C7EE-4FEE-A60D-68CD92F27AF4}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="11_F25DC773A252ABDACC104888095C45085BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0CBCCEF-9122-42A0-BB2E-6EFF705162A8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Wishlist1" sheetId="2" r:id="rId2"/>
     <sheet name="Wishlist2" sheetId="3" r:id="rId3"/>
+    <sheet name="Wishlist3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>Part</t>
   </si>
@@ -221,6 +222,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Reyee WiFi 6 Router AX3200 Wireless Internet High Speed Smart Router</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Reyee-Wireless-Omnidirectional-Antennas-Internet/dp/B09GFP2FHL/ref=sr_1_10?keywords=Wifi%2Brouter%2Blong%2Brange&amp;qid=1701472494&amp;sr=8-10&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://trampaboards.com/vesc-6-mkv-in-cnc-t6-silicone-sealed-aluminium-box-with-genuine-xt90-connectors--vedder-electronic-speed-controller-trampa-special-p-27536.html</t>
+  </si>
+  <si>
+    <t>VESC 6 MkVI</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/HUYUN-Antenna-Module-Wireless-Pigtail/dp/B07DB5VWS1?th=1</t>
+  </si>
+  <si>
+    <t>WLAN Network Adapter PC Antenna</t>
   </si>
 </sst>
 </file>
@@ -754,7 +773,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +882,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,4 +1027,79 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF70BC6-D7C5-4B72-B3FC-EC19F9945E03}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="90.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="67.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2">
+        <v>104.99</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="2">
+        <v>290.25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <f>SUM(B2:B4)</f>
+        <v>403.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix issues with reinforcement learning training and update autoencoder training
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27230"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="241" documentId="11_F25DC773A252ABDACC104888095C45085BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0CBCCEF-9122-42A0-BB2E-6EFF705162A8}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Wishlist2" sheetId="3" r:id="rId3"/>
     <sheet name="Wishlist3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,10 +53,13 @@
     <t>Traxxas Slash Chassis</t>
   </si>
   <si>
+    <t>Complete w/ wheels servo, Velineon motor, possibly do spring replacement in the future</t>
+  </si>
+  <si>
     <t>Traxxas 2S LiPo 5800 mAh</t>
   </si>
   <si>
-    <t>Complete w/ wheels servo, Velineon motor, possibly do spring replacement in the future</t>
+    <t>Slightly bulging - should check to see if not permanently damaged, has XT90 plug</t>
   </si>
   <si>
     <t>Traxxxas EZ-Peak Plus Charger</t>
@@ -80,9 +83,6 @@
     <t>Enertion FOCBOC VESC Motor Controller</t>
   </si>
   <si>
-    <t>Slightly bulging - should check to see if not permanently damaged, has XT90 plug</t>
-  </si>
-  <si>
     <t>Not tested, has USB wire, takes XT90 plug</t>
   </si>
   <si>
@@ -131,96 +131,96 @@
     <t>Price</t>
   </si>
   <si>
+    <t>Buying Link</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bumpers  #6835 &amp; Rear #6836 Bumpers Skid Plate with Mounts </t>
   </si>
   <si>
+    <t>https://www.amazon.com/Bumpers-Compatible-Traxxas-Platinum-Mounts/dp/B093D1GCLY/ref=sr_1_3?keywords=traxxas+slash+bumper&amp;qid=1695671541&amp;sr=8-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sincecam 50KG Brushless Servo Motor 180° Steering Servo Magnetic Metal Gear 1/10 Waterproof </t>
   </si>
   <si>
+    <t>https://www.amazon.com/Sincecam-Brushless-Steering-Induction-Waterproof/dp/B0BMVKHZPJ?th=1</t>
+  </si>
+  <si>
     <t>Sincecam 50kg 12.6V Brushless Servo 3S High Voltage Battery Power Adapter</t>
   </si>
   <si>
+    <t>https://www.amazon.com/Sincecam-Brushless-Voltage-Suitable-SC1250MGX/dp/B0BMVW5DXJ</t>
+  </si>
+  <si>
     <t>Portable Charger 38800mAh,LCD Display Power Bank,4 USB Outputs Battery Pack Backup</t>
   </si>
   <si>
-    <t>Buying Link</t>
+    <t>https://www.amazon.com/Portable-Charger-38800mAh-Charging-Compatible/dp/B09H4GLZXT/ref=sr_1_14?crid=2GYOFTLDQMXKP&amp;keywords=usb%2Bpower%2Bbank%2B3a%2Boutput&amp;qid=1695672928&amp;sprefix=usb%2Bpower%2Bbank%2B3a%2Boutput%2Caps%2C129&amp;sr=8-14&amp;th=1</t>
   </si>
   <si>
     <t xml:space="preserve">NVIDIA Jetson Orin Nano Developer Kit </t>
   </si>
   <si>
-    <t>https://www.amazon.com/Bumpers-Compatible-Traxxas-Platinum-Mounts/dp/B093D1GCLY/ref=sr_1_3?keywords=traxxas+slash+bumper&amp;qid=1695671541&amp;sr=8-3</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Sincecam-Brushless-Steering-Induction-Waterproof/dp/B0BMVKHZPJ?th=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Sincecam-Brushless-Voltage-Suitable-SC1250MGX/dp/B0BMVW5DXJ</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Portable-Charger-38800mAh-Charging-Compatible/dp/B09H4GLZXT/ref=sr_1_14?crid=2GYOFTLDQMXKP&amp;keywords=usb%2Bpower%2Bbank%2B3a%2Boutput&amp;qid=1695672928&amp;sprefix=usb%2Bpower%2Bbank%2B3a%2Boutput%2Caps%2C129&amp;sr=8-14&amp;th=1</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/dp/B0BZJTQ5YP?th=1</t>
   </si>
   <si>
     <t>TOTAL</t>
   </si>
   <si>
+    <t>DC Power Cord 5.5mm x 2.1mm Female to 5.5mm x 2.5mm Male DC Power Adapter Cable</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/COOLM-Female-Adapter-Monitor-Camera/dp/B07FJMX1YR/ref=sr_1_4?crid=1G6NF4G2EG96Q&amp;keywords=5.5%2Bx%2B2.1%2Bto%2B5.5x2.5%2Bbarrel%2Bjack&amp;qid=1701178229&amp;sprefix=5.5%2Bx%2B2.1%2Bto%2B5.5x2.5%2Bbarrel%2Bjack%2Caps%2C103&amp;sr=8-4&amp;th=1</t>
   </si>
   <si>
-    <t>DC Power Cord 5.5mm x 2.1mm Female to 5.5mm x 2.5mm Male DC Power Adapter Cable</t>
+    <t>DC Power Adapter 5.5x2.1mm Female Jack to 5.5x2.5mm Male Plug</t>
   </si>
   <si>
     <t>https://www.amazon.com/ZYAMY-5-5x2-1mm-5-5x2-5mm-Electrical-Converter/dp/B07YWQ9N5S/ref=sr_1_3?crid=1G6NF4G2EG96Q&amp;keywords=5.5%2Bx%2B2.1%2Bto%2B5.5x2.5%2Bbarrel%2Bjack&amp;qid=1701178229&amp;sprefix=5.5%2Bx%2B2.1%2Bto%2B5.5x2.5%2Bbarrel%2Bjack%2Caps%2C103&amp;sr=8-3&amp;th=1</t>
   </si>
   <si>
-    <t>DC Power Adapter 5.5x2.1mm Female Jack to 5.5x2.5mm Male Plug</t>
+    <t>SK hynix Gold P31 500GB PCIe NVMe Gen3 M.2 2280 Internal SSD</t>
   </si>
   <si>
     <t>https://www.amazon.com/dp/B08DK2FB7G?tag=pcpapi-20&amp;linkCode=ogi&amp;th=1&amp;psc=1</t>
   </si>
   <si>
-    <t>SK hynix Gold P31 500GB PCIe NVMe Gen3 M.2 2280 Internal SSD</t>
+    <t>1230PCS Metric Screw Assortment Kit, M2 M3 M4 M5 12.9 Grade Alloy Steel</t>
   </si>
   <si>
     <t>https://www.amazon.com/Zuorery-1230PCS-Assortment-Washers-Upgrade/dp/B0CCXJC8RD/ref=sr_1_3?crid=9TINT5QY4DPF&amp;keywords=m3+m4+screw+kit&amp;qid=1701180792&amp;sprefix=m3+m4+screw+kit%2Caps%2C139&amp;sr=8-3</t>
   </si>
   <si>
-    <t>1230PCS Metric Screw Assortment Kit, M2 M3 M4 M5 12.9 Grade Alloy Steel</t>
-  </si>
-  <si>
     <t>USB C to USB C Cable 1FT, USB C 3.2 Gen 2×2 Right Angle 20Gbps</t>
   </si>
   <si>
     <t>https://www.amazon.com/20Gbps-Transfer-iPhone-Samsung-ARZOPA/dp/B0CFZVW78H/ref=sr_1_15?crid=2GHK8XMIJYPG5&amp;keywords=usb%2Bc%2Bdata%2Bcable%2B1ft&amp;qid=1701182316&amp;sprefix=usb%2Bc%2Bdata%2Bcable%2B1ft%2Caps%2C94&amp;sr=8-15&amp;th=1</t>
   </si>
   <si>
+    <t>16.4Ft(5m) Cable Management Sleeve, 5/8"(16mm) Width PET Black &amp; Gold Cord Protector</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/Bettomshin-16-4X0-05Ft-Expandable-Protector-Television/dp/B08V8YRF47</t>
   </si>
   <si>
-    <t>16.4Ft(5m) Cable Management Sleeve, 5/8"(16mm) Width PET Black &amp; Gold Cord Protector</t>
+    <t>USB C Hub 4 Ports, USB C to USB Hub with 4 USB 3.0, Powered USB C Splitter</t>
   </si>
   <si>
     <t>https://www.amazon.com/UGREEN-Adapter-MacBook-Chromebook-Pixelbook/dp/B07PY87TBD/ref=sr_1_10?crid=3DRCMWEOMPZH5&amp;keywords=compact%2Busb%2Bc%2Bto%2Busb%2Ba%2Bhub%2Bpowered&amp;qid=1701183694&amp;sprefix=compact%2Busb%2Bc%2Bto%2Busb%2Ba%2Bhub%2Bpowered%2Caps%2C101&amp;sr=8-10&amp;th=1</t>
   </si>
   <si>
-    <t>USB C Hub 4 Ports, USB C to USB Hub with 4 USB 3.0, Powered USB C Splitter</t>
+    <t>Cable Zip Ties,400 Pack Black Assorted Sizes 12+8+6+4 Inch</t>
   </si>
   <si>
     <t>https://www.amazon.com/HAVE-ME-TD-Cable-Ties/dp/B08TVLYB3Q/ref=sr_1_3?crid=R8NNKLA59KS4&amp;keywords=zip%2Bties&amp;qid=1701198668&amp;sprefix=zip%2Bties%2Caps%2C130&amp;sr=8-3&amp;th=1</t>
   </si>
   <si>
-    <t>Cable Zip Ties,400 Pack Black Assorted Sizes 12+8+6+4 Inch</t>
+    <t>DP - DisplayPort Display Emulator EDID Emulator Plug 4K</t>
   </si>
   <si>
     <t>https://www.amazon.com/FUERAN-DP-DisplayPort-Emulator-4096x2160/dp/B082J671N2/ref=sr_1_4?crid=2SZVACIHIJMOK&amp;keywords=4k%2Bdisplay%2Bdummy%2Bdisplayport&amp;qid=1701199391&amp;s=electronics&amp;sprefix=4k%2Bdisplay%2Bdummy%2Bdisplayport%2Celectronics%2C55&amp;sr=1-4&amp;th=1</t>
   </si>
   <si>
-    <t>DP - DisplayPort Display Emulator EDID Emulator Plug 4K</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -230,16 +230,16 @@
     <t>https://www.amazon.com/Reyee-Wireless-Omnidirectional-Antennas-Internet/dp/B09GFP2FHL/ref=sr_1_10?keywords=Wifi%2Brouter%2Blong%2Brange&amp;qid=1701472494&amp;sr=8-10&amp;th=1</t>
   </si>
   <si>
+    <t>VESC 6 MkVI</t>
+  </si>
+  <si>
     <t>https://trampaboards.com/vesc-6-mkv-in-cnc-t6-silicone-sealed-aluminium-box-with-genuine-xt90-connectors--vedder-electronic-speed-controller-trampa-special-p-27536.html</t>
   </si>
   <si>
-    <t>VESC 6 MkVI</t>
+    <t>WLAN Network Adapter PC Antenna</t>
   </si>
   <si>
     <t>https://www.amazon.com/HUYUN-Antenna-Module-Wireless-Pigtail/dp/B07DB5VWS1?th=1</t>
-  </si>
-  <si>
-    <t>WLAN Network Adapter PC Antenna</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,10 +326,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,13 +597,13 @@
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="3" max="3" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -626,56 +622,56 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -684,7 +680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -695,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -706,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -714,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -725,7 +721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -736,7 +732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -747,7 +743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -758,7 +754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -776,13 +772,13 @@
       <selection activeCell="A19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="85.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="85.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,56 +786,56 @@
         <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2">
         <v>19.989999999999998</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2">
         <v>81.97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2">
         <v>8.99</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2">
         <v>25.95</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>35</v>
       </c>
       <c r="B6" s="2">
         <v>499.99</v>
@@ -848,18 +844,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="B11" s="2">
         <f>SUM(B1:B6)</f>
         <v>636.89</v>
@@ -885,14 +881,14 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="90.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="67.77734375" customWidth="1"/>
+    <col min="1" max="1" width="90.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,54 +896,54 @@
         <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2">
         <v>5.89</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2">
         <v>6.99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2">
         <v>45.53</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2">
         <v>17.989999999999998</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -958,56 +954,56 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2">
         <v>10.99</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2">
         <v>14.99</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2">
         <v>5.99</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2">
         <v>29.99</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="B13" s="2">
         <f>SUM(B2:B10)</f>
         <v>153.34999999999997</v>
@@ -1037,14 +1033,14 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="90.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="67.77734375" customWidth="1"/>
+    <col min="1" max="1" width="90.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,10 +1048,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1066,34 +1062,34 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2">
         <v>290.25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2">
         <v>7.99</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="B6" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="B7" s="2">
         <f>SUM(B2:B4)</f>
         <v>403.23</v>

</xml_diff>

<commit_message>
another week of journal reports
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0f92f3d012b9fa0/Documents/Senior_Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="11_F25DC773A252ABDACC104888095C45085BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0CBCCEF-9122-42A0-BB2E-6EFF705162A8}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="11_F25DC773A252ABDACC104888095C45085BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ED7762F-9336-4273-8EF0-4CEED77BC5CB}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Wishlist1" sheetId="2" r:id="rId2"/>
     <sheet name="Wishlist2" sheetId="3" r:id="rId3"/>
     <sheet name="Wishlist3" sheetId="4" r:id="rId4"/>
+    <sheet name="Wishlist4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>Part</t>
   </si>
@@ -240,6 +241,27 @@
   </si>
   <si>
     <t>https://www.amazon.com/HUYUN-Antenna-Module-Wireless-Pigtail/dp/B07DB5VWS1?th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B07QMJ8XGF/ref=sspa_dk_detail_0?psc=1&amp;pd_rd_i=B07QMJ8XGF&amp;pd_rd_w=hYV87&amp;pf_rd_p=45a72588-80f7-4414-9851-786f6c16d42b&amp;pd_rd_wg=d2yzO&amp;pf_rd_r=HY77N499JKE03N2HRHF5&amp;pd_rd_r=354d7a25-92eb-4811-9576-3f149695dea8&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExMVFFTkQ0U0pDNllWJmVuY3J5cHRlZElkPUEwOTI3NzI5MUE5RENJSjRMV1JHUSZlbmNyeXB0ZWRBZElkPUEwNTMyNDEwM0NIN0pQQ1M2STRJTCZ3aWRnZXROYW1lPXNwX2RldGFpbCZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=</t>
+  </si>
+  <si>
+    <t>3pcs XT90 Female Connector Adapter Plug</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/JFtech-Bullet-Connector-Conversion-Adapter/dp/B07BGD3MY2/ref=sr_1_4?crid=JGB4E04KKQJQ&amp;keywords=Bullet+Adapter+%284mm+Male+to+3.5mm+Female%29&amp;qid=1706647534&amp;s=toys-and-games&amp;sprefix=bullet+adapter+4mm+male+to+3.5mm+female+%2Ctoys-and-games%2C207&amp;sr=1-4</t>
+  </si>
+  <si>
+    <t>Male Bullet Connector to 3.5mm Female Bullet Connector Gold Plug Conversion</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Monoprice-Power-Cord-5-15P-3-Prong/dp/B08BXM5CGB/ref=sr_1_3?crid=2D2VAYV8B7RZI&amp;keywords=%2C%2BNEMA%2B5-15P%2Bto%2BC5%2B6%2Binches&amp;qid=1706647701&amp;s=electronics&amp;sprefix=nema%2B5-15p%2Bto%2Bc5%2B6%2Binc%2Celectronics%2C266&amp;sr=1-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Power Cord - NEMA 5-15P to IEC 60320 C5 1ft</t>
   </si>
 </sst>
 </file>
@@ -249,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +348,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -597,13 +623,13 @@
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="3" max="3" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -625,7 +651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -636,7 +662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -647,7 +673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -658,7 +684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -669,7 +695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -680,7 +706,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -691,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -702,7 +728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -710,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -721,7 +747,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -732,7 +758,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -743,7 +769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -754,7 +780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -772,13 +798,13 @@
       <selection activeCell="A19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="85.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="85.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +815,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -800,7 +826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -811,7 +837,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -822,7 +848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -833,7 +859,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -844,18 +870,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <f>SUM(B1:B6)</f>
         <v>636.89</v>
@@ -877,18 +903,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0D9DD-E951-4200-9E8B-67C4AB29FC85}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="90.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="2"/>
-    <col min="3" max="3" width="67.7109375" customWidth="1"/>
+    <col min="1" max="1" width="90.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -910,7 +936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -921,7 +947,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -932,7 +958,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -943,7 +969,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -954,7 +980,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -965,7 +991,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -976,7 +1002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -987,7 +1013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -998,12 +1024,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <f>SUM(B2:B10)</f>
         <v>153.34999999999997</v>
@@ -1033,14 +1059,14 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="90.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="2"/>
-    <col min="3" max="3" width="67.7109375" customWidth="1"/>
+    <col min="1" max="1" width="90.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1077,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1062,7 +1088,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1073,7 +1099,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1084,12 +1110,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f>SUM(B2:B4)</f>
         <v>403.23</v>
@@ -1098,4 +1124,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476CACAD-AC42-4B54-83EC-42059881394A}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="68.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10.99</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <f>SUM(B2:B4)</f>
+        <v>23.36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.amazon.com/JFtech-Bullet-Connector-Conversion-Adapter/dp/B07BGD3MY2/ref=sr_1_4?crid=JGB4E04KKQJQ&amp;keywords=Bullet+Adapter+%284mm+Male+to+3.5mm+Female%29&amp;qid=1706647534&amp;s=toys-and-games&amp;sprefix=bullet+adapter+4mm+male+to+3.5mm+female+%2Ctoys-and-games%2C207&amp;sr=1-4" xr:uid="{445010D0-13B5-4B6C-B894-DA9D639B0AD6}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{2A36705D-048D-4F9E-8417-FEBEF7F87BA8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>